<commit_message>
Fix trend line baseline to use actual mean at center year
</commit_message>
<xml_diff>
--- a/tables_and_figures/output/rmse_trend_regression_by_variable.xlsx
+++ b/tables_and_figures/output/rmse_trend_regression_by_variable.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,32 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Class</t>
+          <t>Slope</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Slope</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Intercept</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>R_squared</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
           <t>p_value</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>n_years</t>
         </is>
       </c>
     </row>
@@ -476,25 +456,11 @@
           <t>Veteran Status</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Demographic</t>
-        </is>
+      <c r="B2" t="n">
+        <v>-0.134841301067288</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.1371183822482574</v>
-      </c>
-      <c r="D2" t="n">
-        <v>279.9294646917022</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.7966417349107129</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.001203719133328357</v>
-      </c>
-      <c r="G2" t="n">
-        <v>9</v>
+        <v>0.00135846697049377</v>
       </c>
     </row>
     <row r="3">
@@ -503,79 +469,37 @@
           <t>Family Income</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Demographic</t>
-        </is>
+      <c r="B3" t="n">
+        <v>0.2584828359824106</v>
       </c>
       <c r="C3" t="n">
-        <v>0.256192616370782</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-510.8538336705582</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.694108151500632</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.005286936901865157</v>
-      </c>
-      <c r="G3" t="n">
-        <v>9</v>
+        <v>0.0192849003679574</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>State Representative</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Candidate Choice</t>
-        </is>
+          <t>Voting Method</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.137223807092183</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2545756451891081</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-505.3577687822998</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.4816676781440163</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.03807799787749788</v>
-      </c>
-      <c r="G4" t="n">
-        <v>9</v>
+        <v>0.04497397374979856</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Voting Method</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Voting Administration</t>
-        </is>
+          <t>State Representative</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.1116634092427386</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1272206067540947</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-251.2210233108093</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.3848324103676456</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.07468176592276468</v>
-      </c>
-      <c r="G5" t="n">
-        <v>9</v>
+        <v>0.1229602268622791</v>
       </c>
     </row>
     <row r="6">
@@ -584,25 +508,11 @@
           <t>Employment Status</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Demographic</t>
-        </is>
+      <c r="B6" t="n">
+        <v>0.2152019105524243</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1719996019714637</v>
-      </c>
-      <c r="D6" t="n">
-        <v>-335.3334533844215</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.2478107340339885</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.1726560104415032</v>
-      </c>
-      <c r="G6" t="n">
-        <v>9</v>
+        <v>0.1486843722550557</v>
       </c>
     </row>
     <row r="7">
@@ -611,25 +521,11 @@
           <t>Union Membership</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Demographic</t>
-        </is>
+      <c r="B7" t="n">
+        <v>0.08367787393634148</v>
       </c>
       <c r="C7" t="n">
-        <v>0.06497257747459843</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-125.406893381655</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.2124954386895667</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.2117173631184056</v>
-      </c>
-      <c r="G7" t="n">
-        <v>9</v>
+        <v>0.1494887215625006</v>
       </c>
     </row>
     <row r="8">
@@ -638,25 +534,11 @@
           <t>U.S. House</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Candidate Choice</t>
-        </is>
+      <c r="B8" t="n">
+        <v>0.09288080445776516</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1044944683667673</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-201.3632056075754</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.1016379248023789</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.4030552981281471</v>
-      </c>
-      <c r="G8" t="n">
-        <v>9</v>
+        <v>0.3989869415835802</v>
       </c>
     </row>
     <row r="9">
@@ -665,25 +547,11 @@
           <t>State Senator</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Candidate Choice</t>
-        </is>
+      <c r="B9" t="n">
+        <v>-0.02002032986058871</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.09375979781758607</v>
-      </c>
-      <c r="D9" t="n">
-        <v>197.4074243642994</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.03769833979026427</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.6166754428368786</v>
-      </c>
-      <c r="G9" t="n">
-        <v>9</v>
+        <v>0.8541625635049479</v>
       </c>
     </row>
   </sheetData>

</xml_diff>